<commit_message>
Updated example according to the metamodel changes
</commit_message>
<xml_diff>
--- a/be.uantwerpen.msdl.icm.cases.agv2/Intent Table.xlsx
+++ b/be.uantwerpen.msdl.icm.cases.agv2/Intent Table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\msdl\agv\be.uantwerpen.msdl.icm.cases.agv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="new_IntentTable" localSheetId="0">Sheet1!$A$1:$S$16</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -312,8 +313,36 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -594,9 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>